<commit_message>
Turning ints to strings so that the report can serialize correctly. Since strings are nullable, the report can correctly print nothing when there's no data for particular properties
</commit_message>
<xml_diff>
--- a/NibrsXmlGenerator/NibrsXmlGenerator/NIBRSXSD/docs/nibrsCodesTables.xlsx
+++ b/NibrsXmlGenerator/NibrsXmlGenerator/NIBRSXSD/docs/nibrsCodesTables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\ITMS-ETSU\Projects\Enterprise XML Development\UCR NIBRS XML Development\IEPD\NIBRS_IEPD_4_0\NIBRS IEPD 4_0\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\checkouts\NIBRSXML\NibrsXmlGenerator\NibrsXmlGenerator\NIBRSXSD\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="22380" windowHeight="11370" tabRatio="731"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="22380" windowHeight="11370" tabRatio="731" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Code List Index" sheetId="152" r:id="rId1"/>
@@ -2592,7 +2592,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2602,6 +2602,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2810,7 +2816,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -3113,6 +3119,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -3435,7 +3447,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3650,7 +3664,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3925,7 +3939,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B18" sqref="A17:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4154,8 +4168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4753,7 +4767,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4916,7 +4930,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A38" sqref="A38:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5386,7 +5400,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5463,7 +5477,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5921,7 +5935,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6014,7 +6028,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6093,7 +6107,7 @@
   <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6850,7 +6864,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7290,7 +7304,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7729,7 +7743,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8146,7 +8160,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8494,7 +8508,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9323,7 +9337,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9365,10 +9379,10 @@
       <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:6" s="9" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="120" t="s">
         <v>499</v>
       </c>
       <c r="C4" s="19"/>
@@ -9413,10 +9427,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="119" t="s">
         <v>223</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="120" t="s">
         <v>500</v>
       </c>
     </row>
@@ -9469,10 +9483,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="55" t="s">
+      <c r="A16" s="119" t="s">
         <v>206</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="120" t="s">
         <v>502</v>
       </c>
     </row>
@@ -9511,7 +9525,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B20" sqref="A20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9705,8 +9719,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="A4:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Builder classes have been created up to Location (exclusive). Some todos have been added to the task list for ReportBuilder.cs and SubmissionBuilder.cs. Some classes were renamed from NIBRS... to Nibrs...
</commit_message>
<xml_diff>
--- a/NibrsXmlGenerator/NibrsXmlGenerator/NIBRSXSD/docs/nibrsCodesTables.xlsx
+++ b/NibrsXmlGenerator/NibrsXmlGenerator/NIBRSXSD/docs/nibrsCodesTables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="22380" windowHeight="11370" tabRatio="731" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="22380" windowHeight="11370" tabRatio="731" firstSheet="15" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Code List Index" sheetId="152" r:id="rId1"/>
@@ -122,7 +122,7 @@
     <definedName name="Start8">#REF!</definedName>
     <definedName name="Start9">SubstanceUnitCode!$D$1</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -2993,6 +2993,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3119,12 +3125,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -3448,7 +3448,7 @@
   <dimension ref="A1:A32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3676,19 +3676,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>677</v>
       </c>
-      <c r="B1" s="85"/>
+      <c r="B1" s="87"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="98" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="97"/>
+      <c r="B2" s="99"/>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -3778,7 +3778,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3791,19 +3791,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>671</v>
       </c>
-      <c r="B1" s="80"/>
+      <c r="B1" s="82"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="83" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="82"/>
+      <c r="B2" s="84"/>
       <c r="C2" s="61"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3952,20 +3952,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="100" t="s">
         <v>621</v>
       </c>
-      <c r="B1" s="98"/>
+      <c r="B1" s="100"/>
       <c r="C1" s="6"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="101" t="s">
         <v>270</v>
       </c>
-      <c r="B2" s="99"/>
+      <c r="B2" s="101"/>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.2">
@@ -4060,19 +4060,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>622</v>
       </c>
-      <c r="B1" s="85"/>
+      <c r="B1" s="87"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="102" t="s">
         <v>280</v>
       </c>
-      <c r="B2" s="100"/>
+      <c r="B2" s="102"/>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -4180,20 +4180,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="85" t="s">
         <v>628</v>
       </c>
-      <c r="B1" s="83"/>
+      <c r="B1" s="85"/>
       <c r="C1" s="4"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="103" t="s">
         <v>629</v>
       </c>
-      <c r="B2" s="101"/>
+      <c r="B2" s="103"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="51" t="s">
@@ -4767,7 +4767,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4780,22 +4780,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>766</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="104" t="s">
         <v>365</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
     </row>
     <row r="3" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
@@ -4942,20 +4942,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="85" t="s">
         <v>763</v>
       </c>
-      <c r="B1" s="83"/>
+      <c r="B1" s="85"/>
       <c r="C1" s="48"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="103" t="s">
         <v>678</v>
       </c>
-      <c r="B2" s="101"/>
+      <c r="B2" s="103"/>
       <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5410,17 +5410,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="105" t="s">
         <v>679</v>
       </c>
-      <c r="B1" s="103"/>
+      <c r="B1" s="105"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="104"/>
-      <c r="B2" s="104"/>
+      <c r="A2" s="106"/>
+      <c r="B2" s="106"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
@@ -5476,8 +5476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D39" sqref="D4:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5490,22 +5490,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>644</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="104" t="s">
         <v>260</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
     </row>
     <row r="3" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
@@ -5528,7 +5528,10 @@
       <c r="C4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="15"/>
+      <c r="D4" s="15" t="str">
+        <f>"{ """&amp;C4&amp;""", BiasMotivationCode."&amp;SUBSTITUTE(A4, " ", "_")&amp;".NibrsCode() },"</f>
+        <v>{ "11", BiasMotivationCode.ANTIWHITE.NibrsCode() },</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
@@ -5540,7 +5543,10 @@
       <c r="C5" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="15"/>
+      <c r="D5" s="15" t="str">
+        <f t="shared" ref="D5:D39" si="0">"{ """&amp;C5&amp;""", BiasMotivationCode."&amp;SUBSTITUTE(A5, " ", "_")&amp;".NibrsCode() },"</f>
+        <v>{ "12", BiasMotivationCode.ANTIBLACK_AFRICAN_AMERICAN.NibrsCode() },</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
@@ -5552,6 +5558,10 @@
       <c r="C6" s="8" t="s">
         <v>170</v>
       </c>
+      <c r="D6" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "13", BiasMotivationCode.ANTIAMERICAN_INDIAN__ALASKAN_NATIVE.NibrsCode() },</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
@@ -5563,6 +5573,10 @@
       <c r="C7" s="8" t="s">
         <v>171</v>
       </c>
+      <c r="D7" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "14", BiasMotivationCode.ANTIASIAN.NibrsCode() },</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
@@ -5574,6 +5588,10 @@
       <c r="C8" s="8" t="s">
         <v>172</v>
       </c>
+      <c r="D8" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "15", BiasMotivationCode.ANTIMULTIRACIAL_GROUP.NibrsCode() },</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -5585,6 +5603,10 @@
       <c r="C9" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="D9" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "16", BiasMotivationCode.ANTINATIVEHAWAIIAN_OTHERPACIFICISLANDER.NibrsCode() },</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -5596,6 +5618,10 @@
       <c r="C10" s="8" t="s">
         <v>174</v>
       </c>
+      <c r="D10" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "21", BiasMotivationCode.ANTIJEWISH.NibrsCode() },</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
@@ -5607,6 +5633,10 @@
       <c r="C11" s="8" t="s">
         <v>175</v>
       </c>
+      <c r="D11" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "22", BiasMotivationCode.ANTICATHOLIC.NibrsCode() },</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
@@ -5618,6 +5648,10 @@
       <c r="C12" s="8" t="s">
         <v>176</v>
       </c>
+      <c r="D12" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "23", BiasMotivationCode.ANTIPROTESTANT.NibrsCode() },</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
@@ -5629,6 +5663,10 @@
       <c r="C13" s="8" t="s">
         <v>177</v>
       </c>
+      <c r="D13" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "24", BiasMotivationCode.ANTIISLAMIC.NibrsCode() },</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
@@ -5640,6 +5678,10 @@
       <c r="C14" s="8" t="s">
         <v>178</v>
       </c>
+      <c r="D14" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "25", BiasMotivationCode.ANTIOTHER_RELIGION.NibrsCode() },</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -5651,6 +5693,10 @@
       <c r="C15" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="D15" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "26", BiasMotivationCode.ANTIMULTIRELIGIOUS_GROUP.NibrsCode() },</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
@@ -5662,8 +5708,12 @@
       <c r="C16" s="8" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "27", BiasMotivationCode.ANTIATHEIST_AGNOSTIC.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="55" t="s">
         <v>687</v>
       </c>
@@ -5673,8 +5723,12 @@
       <c r="C17" s="55" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "28", BiasMotivationCode.ANTIMORMON.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="55" t="s">
         <v>706</v>
       </c>
@@ -5684,8 +5738,12 @@
       <c r="C18" s="55" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "29", BiasMotivationCode.ANTIJEHOVAHWITNESS.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="55" t="s">
         <v>688</v>
       </c>
@@ -5695,8 +5753,12 @@
       <c r="C19" s="55" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "31", BiasMotivationCode.ANTIARAB.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>709</v>
       </c>
@@ -5706,8 +5768,12 @@
       <c r="C20" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "32", BiasMotivationCode.ANTIHISPANIC_LATINO.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>716</v>
       </c>
@@ -5717,8 +5783,12 @@
       <c r="C21" s="8" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "33", BiasMotivationCode.ANTIOTHER_ETHNICITY_NATIONAL_ORIGIN.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>707</v>
       </c>
@@ -5728,8 +5798,12 @@
       <c r="C22" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "41", BiasMotivationCode.ANTIMALE_HOMOSEXUAL.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>708</v>
       </c>
@@ -5739,8 +5813,12 @@
       <c r="C23" s="8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "42", BiasMotivationCode.ANTIFEMALE_HOMOSEXUAL.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>710</v>
       </c>
@@ -5750,8 +5828,12 @@
       <c r="C24" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "43", BiasMotivationCode.ANTIHOMOSEXUAL.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>689</v>
       </c>
@@ -5761,8 +5843,12 @@
       <c r="C25" s="8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "44", BiasMotivationCode.ANTIHETEROSEXUAL.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>690</v>
       </c>
@@ -5772,8 +5858,12 @@
       <c r="C26" s="8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "45", BiasMotivationCode.ANTIBISEXUAL.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>701</v>
       </c>
@@ -5783,8 +5873,12 @@
       <c r="C27" s="8" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "51", BiasMotivationCode.ANTIPHYSICAL_DISABILITY.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>702</v>
       </c>
@@ -5794,8 +5888,12 @@
       <c r="C28" s="8" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "52", BiasMotivationCode.ANTIMENTAL_DISABILITY.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>691</v>
       </c>
@@ -5805,8 +5903,12 @@
       <c r="C29" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "61", BiasMotivationCode.ANTIMALE.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>692</v>
       </c>
@@ -5816,8 +5918,12 @@
       <c r="C30" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "62", BiasMotivationCode.ANTIFEMALE.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>693</v>
       </c>
@@ -5827,8 +5933,12 @@
       <c r="C31" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "71", BiasMotivationCode.ANTITRANSGENDER.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>713</v>
       </c>
@@ -5838,8 +5948,12 @@
       <c r="C32" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "72", BiasMotivationCode.ANTIGENDER_NONCONFORMING.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="66" t="s">
         <v>712</v>
       </c>
@@ -5849,8 +5963,12 @@
       <c r="C33" s="66">
         <v>81</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "81", BiasMotivationCode.ANTIEASTERNORTHODOX.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="66" t="s">
         <v>703</v>
       </c>
@@ -5860,8 +5978,12 @@
       <c r="C34" s="66">
         <v>82</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "82", BiasMotivationCode.ANTIOTHER_CHRISTIAN.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="66" t="s">
         <v>714</v>
       </c>
@@ -5871,8 +5993,12 @@
       <c r="C35" s="66">
         <v>83</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "83", BiasMotivationCode.ANTIBUDDHIST.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="66" t="s">
         <v>694</v>
       </c>
@@ -5882,8 +6008,12 @@
       <c r="C36" s="66">
         <v>84</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "84", BiasMotivationCode.ANTIHINDU.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="66" t="s">
         <v>695</v>
       </c>
@@ -5893,8 +6023,12 @@
       <c r="C37" s="66">
         <v>85</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "85", BiasMotivationCode.ANTISIKH.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>711</v>
       </c>
@@ -5904,8 +6038,12 @@
       <c r="C38" s="8" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "88", BiasMotivationCode.NONE.NibrsCode() },</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>715</v>
       </c>
@@ -5914,6 +6052,10 @@
       </c>
       <c r="C39" s="8" t="s">
         <v>402</v>
+      </c>
+      <c r="D39" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v>{ "99", BiasMotivationCode.UNKNOWN.NibrsCode() },</v>
       </c>
     </row>
   </sheetData>
@@ -5948,20 +6090,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="100" t="s">
         <v>623</v>
       </c>
-      <c r="B1" s="98"/>
+      <c r="B1" s="100"/>
       <c r="C1" s="6"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="101" t="s">
         <v>277</v>
       </c>
-      <c r="B2" s="99"/>
+      <c r="B2" s="101"/>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6041,19 +6183,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="78" t="s">
         <v>670</v>
       </c>
-      <c r="B1" s="76"/>
+      <c r="B1" s="78"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="79" t="s">
         <v>207</v>
       </c>
-      <c r="B2" s="78"/>
+      <c r="B2" s="80"/>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6120,19 +6262,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>762</v>
       </c>
-      <c r="B1" s="85"/>
+      <c r="B1" s="87"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="90" t="s">
         <v>303</v>
       </c>
-      <c r="B2" s="89"/>
+      <c r="B2" s="91"/>
       <c r="C2" s="16"/>
       <c r="D2" s="15"/>
     </row>
@@ -6800,19 +6942,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="100" t="s">
         <v>627</v>
       </c>
-      <c r="B1" s="98"/>
+      <c r="B1" s="100"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="101" t="s">
         <v>300</v>
       </c>
-      <c r="B2" s="99"/>
+      <c r="B2" s="101"/>
     </row>
     <row r="3" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
@@ -6875,21 +7017,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="107" t="s">
         <v>719</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
       <c r="E1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="108" t="s">
         <v>730</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
@@ -6967,19 +7109,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>731</v>
       </c>
-      <c r="B1" s="85"/>
+      <c r="B1" s="87"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="90" t="s">
         <v>252</v>
       </c>
-      <c r="B2" s="89"/>
+      <c r="B2" s="91"/>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -7049,19 +7191,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="110" t="s">
         <v>617</v>
       </c>
-      <c r="B1" s="108"/>
+      <c r="B1" s="110"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="111" t="s">
         <v>379</v>
       </c>
-      <c r="B2" s="109"/>
+      <c r="B2" s="111"/>
       <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:4" s="38" customFormat="1" x14ac:dyDescent="0.2">
@@ -7156,19 +7298,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>732</v>
       </c>
-      <c r="B1" s="85"/>
+      <c r="B1" s="87"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="96" t="s">
         <v>366</v>
       </c>
-      <c r="B2" s="95"/>
+      <c r="B2" s="97"/>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.2">
@@ -7235,19 +7377,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>616</v>
       </c>
-      <c r="B1" s="85"/>
+      <c r="B1" s="87"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="93" t="s">
         <v>372</v>
       </c>
-      <c r="B2" s="110"/>
+      <c r="B2" s="112"/>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -7313,19 +7455,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="105" t="s">
         <v>733</v>
       </c>
-      <c r="B1" s="103"/>
+      <c r="B1" s="105"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="113" t="s">
         <v>642</v>
       </c>
-      <c r="B2" s="112"/>
+      <c r="B2" s="114"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="59" t="s">
@@ -7382,20 +7524,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>620</v>
       </c>
-      <c r="B1" s="85"/>
+      <c r="B1" s="87"/>
       <c r="C1"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="115" t="s">
         <v>229</v>
       </c>
-      <c r="B2" s="114"/>
+      <c r="B2" s="116"/>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -7532,20 +7674,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>765</v>
       </c>
-      <c r="B1" s="85"/>
+      <c r="B1" s="87"/>
       <c r="C1" s="12"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="117" t="s">
         <v>204</v>
       </c>
-      <c r="B2" s="115"/>
+      <c r="B2" s="117"/>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -7756,19 +7898,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="81" t="s">
         <v>671</v>
       </c>
-      <c r="B1" s="80"/>
+      <c r="B1" s="82"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="83" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="82"/>
+      <c r="B2" s="84"/>
       <c r="C2" s="61"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7914,19 +8056,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="105" t="s">
         <v>734</v>
       </c>
-      <c r="B1" s="103"/>
+      <c r="B1" s="105"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="118" t="s">
         <v>373</v>
       </c>
-      <c r="B2" s="117"/>
+      <c r="B2" s="119"/>
       <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:4" s="38" customFormat="1" x14ac:dyDescent="0.2">
@@ -8059,19 +8201,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>624</v>
       </c>
-      <c r="B1" s="85"/>
+      <c r="B1" s="87"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="90" t="s">
         <v>281</v>
       </c>
-      <c r="B2" s="89"/>
+      <c r="B2" s="91"/>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -8171,18 +8313,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="120" t="s">
         <v>753</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
+      <c r="B1" s="120"/>
+      <c r="C1" s="120"/>
     </row>
     <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="108" t="s">
         <v>735</v>
       </c>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="69" t="s">
@@ -8520,20 +8662,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="85" t="s">
         <v>626</v>
       </c>
-      <c r="B1" s="83"/>
+      <c r="B1" s="85"/>
       <c r="C1" s="48"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="86" t="s">
         <v>625</v>
       </c>
-      <c r="B2" s="84"/>
+      <c r="B2" s="86"/>
       <c r="C2" s="49"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8592,19 +8734,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>674</v>
       </c>
-      <c r="B1" s="85"/>
+      <c r="B1" s="87"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>675</v>
       </c>
-      <c r="B2" s="87"/>
+      <c r="B2" s="89"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
@@ -8668,19 +8810,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>764</v>
       </c>
-      <c r="B1" s="85"/>
+      <c r="B1" s="87"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="90" t="s">
         <v>303</v>
       </c>
-      <c r="B2" s="89"/>
+      <c r="B2" s="91"/>
       <c r="C2" s="16"/>
       <c r="D2" s="15"/>
     </row>
@@ -9350,10 +9492,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>717</v>
       </c>
-      <c r="B1" s="90"/>
+      <c r="B1" s="92"/>
       <c r="C1"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
@@ -9361,10 +9503,10 @@
       <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="93" t="s">
         <v>219</v>
       </c>
-      <c r="B2" s="91"/>
+      <c r="B2" s="93"/>
       <c r="C2" s="18"/>
       <c r="F2" s="17"/>
     </row>
@@ -9379,10 +9521,10 @@
       <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:6" s="9" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="119" t="s">
+      <c r="A4" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="120" t="s">
+      <c r="B4" s="77" t="s">
         <v>499</v>
       </c>
       <c r="C4" s="19"/>
@@ -9427,10 +9569,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="119" t="s">
+      <c r="A9" s="76" t="s">
         <v>223</v>
       </c>
-      <c r="B9" s="120" t="s">
+      <c r="B9" s="77" t="s">
         <v>500</v>
       </c>
     </row>
@@ -9483,10 +9625,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="119" t="s">
+      <c r="A16" s="76" t="s">
         <v>206</v>
       </c>
-      <c r="B16" s="120" t="s">
+      <c r="B16" s="77" t="s">
         <v>502</v>
       </c>
     </row>
@@ -9536,19 +9678,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="85" t="s">
         <v>618</v>
       </c>
-      <c r="B1" s="83"/>
+      <c r="B1" s="85"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="94" t="s">
         <v>619</v>
       </c>
-      <c r="B2" s="93"/>
+      <c r="B2" s="95"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -9719,8 +9861,8 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="A4:B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9733,19 +9875,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>676</v>
       </c>
-      <c r="B1" s="85"/>
+      <c r="B1" s="87"/>
       <c r="D1" s="5" t="s">
         <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="96" t="s">
         <v>289</v>
       </c>
-      <c r="B2" s="95"/>
+      <c r="B2" s="97"/>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>